<commit_message>
added coding status info in supplementary table
</commit_message>
<xml_diff>
--- a/Supplementary_files/Supplementary_Tables_1-6.xlsx
+++ b/Supplementary_files/Supplementary_Tables_1-6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\01_Current_reserach\01_Projects\01_PhD_project\isi_t2d\Supplementary_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC5A20C-E80F-4ED3-A4A1-12C0DC198457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6AB0EF9-2C2B-40ED-A7D0-D89A86A31F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8510" yWindow="-14510" windowWidth="34620" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>

</xml_diff>